<commit_message>
close #42 people drop cardbag now. gameshop price decide by item value
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassic\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="GameShop" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -41,17 +44,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>价格</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
     <t>Shelf</t>
-  </si>
-  <si>
-    <t>Price</t>
   </si>
   <si>
     <t>Id</t>
@@ -59,6 +55,18 @@
   </si>
   <si>
     <t>ItemId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具名</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -745,6 +753,524 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="材料"/>
+      <sheetName val="任务"/>
+      <sheetName val="其他"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>名字</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>string</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Name</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>新手礼包</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>随机卡牌（无）</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>随机卡牌（水）</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>随机卡牌（风）</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>随机卡牌（地）</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>随机卡牌（火）</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>随机卡牌（光）</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>随机卡牌（暗）</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12" t="str">
+            <v>资源袋(植物)</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>资源袋(鱼)</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>资源袋(矿石)</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v>蓝色卡包</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>黄色卡包</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v>红色卡包</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18" t="str">
+            <v>木材补给车</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19" t="str">
+            <v>矿石补给车</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20" t="str">
+            <v>水银补给车</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21" t="str">
+            <v>红宝石补给车</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>硫磺补给车</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v>水晶补给车</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v>初始资源包</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>金币</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>小型魔法药剂</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>中型魔法药剂</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>大型魔法药剂</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29" t="str">
+            <v>小型恢复药剂</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30" t="str">
+            <v>中型恢复药剂</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31" t="str">
+            <v>大型恢复药剂</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32" t="str">
+            <v>小型活力药剂</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33" t="str">
+            <v>中型活力药剂</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34" t="str">
+            <v>大型活力药剂</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35" t="str">
+            <v>随机幻兽卡</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36" t="str">
+            <v>随机武器卡</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37" t="str">
+            <v>随机魔法卡</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="B38" t="str">
+            <v>符文-查姆</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39" t="str">
+            <v>符文-普尔</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="B40" t="str">
+            <v>符文-艾尔</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41" t="str">
+            <v>小型药剂-命</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42" t="str">
+            <v>药剂-命</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43" t="str">
+            <v>大型药剂-命</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="B44" t="str">
+            <v>经验之书</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="B45" t="str">
+            <v>能量之书</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="B46" t="str">
+            <v>战斗药水</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="B47" t="str">
+            <v>守护药水</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="B48" t="str">
+            <v>法术药水</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="B49" t="str">
+            <v>技巧药水</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="B50" t="str">
+            <v>速度药水</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="B51" t="str">
+            <v>幸运药水</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="B52" t="str">
+            <v>体质药水</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="B53" t="str">
+            <v>生存药水</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="B54" t="str">
+            <v>体力药水</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="B55" t="str">
+            <v>猛兽卡片</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="B56" t="str">
+            <v>战斧卡片</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="B57" t="str">
+            <v>火焰卡片</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="B58" t="str">
+            <v>名片-塞尼斯</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="B59" t="str">
+            <v>名片-塞巴斯恰恩</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="B60" t="str">
+            <v>名片-科迪</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="B61" t="str">
+            <v>名片-威阿伊丁</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="B62" t="str">
+            <v>名片-奥莱伊李</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="B63" t="str">
+            <v>名片-米兰达</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="B64" t="str">
+            <v>名片-盖露贝尔</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="B65" t="str">
+            <v>名片-贝露凯伊鲁</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="B66" t="str">
+            <v>名片-雷洛比克</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="B67" t="str">
+            <v>名片-巴鲁迪亚斯</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="B68" t="str">
+            <v>名片-武藤游戏</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="B69" t="str">
+            <v>名片-城之内</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="B70" t="str">
+            <v>名片-海马懒人</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="B71" t="str">
+            <v>名片-内芙妮</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="B72" t="str">
+            <v>名片-塔妮丝</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="B73" t="str">
+            <v>名片-卢卡</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="B74" t="str">
+            <v>名片-艾斯特尔</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="B75" t="str">
+            <v>名片-萨恩</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="B76" t="str">
+            <v>名片-玛莎</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="B77" t="str">
+            <v>名片-阿特罗姆</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="B78" t="str">
+            <v>名片-泽诺</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="B79" t="str">
+            <v>名片-拉凯尔</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="B80" t="str">
+            <v>名片-纳尔萨斯</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="B81" t="str">
+            <v>名片-纳隆</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="B82" t="str">
+            <v>名片-维加</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="B83" t="str">
+            <v>名片-诺德</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="B84" t="str">
+            <v>名片-那那美</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="B85" t="str">
+            <v>名片-弗兰克</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="B86" t="str">
+            <v>名片-维克托</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="B87" t="str">
+            <v>名片-洛克</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="B88" t="str">
+            <v>名片-谢拉</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="B89" t="str">
+            <v>名片-克莱布</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="B90" t="str">
+            <v>名片-蔡</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="B91" t="str">
+            <v>名片-约修亚</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="B92" t="str">
+            <v>名片-艾斯蒂尔</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="B93" t="str">
+            <v>种子-豌豆</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="B94" t="str">
+            <v>种子-玉米</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="B95" t="str">
+            <v>种子-苹果</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="B96" t="str">
+            <v>种子-蓝莓</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="B97" t="str">
+            <v>作物-豌豆</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="B98" t="str">
+            <v>作物-豌豆</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="B99" t="str">
+            <v>作物-苹果</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="B100" t="str">
+            <v>作物-蓝莓</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E46" totalsRowShown="0">
   <autoFilter ref="A1:E46"/>
@@ -753,7 +1279,7 @@
     <tableColumn id="2" name="ItemId"/>
     <tableColumn id="3" name="Type"/>
     <tableColumn id="4" name="Shelf"/>
-    <tableColumn id="5" name="Price"/>
+    <tableColumn id="5" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1049,7 +1575,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1059,19 +1585,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1088,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1105,7 +1631,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -1121,8 +1647,9 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>50</v>
+      <c r="E4" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>猛兽卡片</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -1138,8 +1665,9 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>100</v>
+      <c r="E5" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>战斧卡片</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1155,8 +1683,9 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>200</v>
+      <c r="E6" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>火焰卡片</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -1172,8 +1701,9 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>50</v>
+      <c r="E7" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机卡牌（无）</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -1189,8 +1719,9 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8">
-        <v>50</v>
+      <c r="E8" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机卡牌（水）</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -1206,8 +1737,9 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9">
-        <v>50</v>
+      <c r="E9" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机卡牌（风）</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -1223,8 +1755,9 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10">
-        <v>50</v>
+      <c r="E10" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机卡牌（地）</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -1240,8 +1773,9 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11">
-        <v>50</v>
+      <c r="E11" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机卡牌（火）</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -1257,8 +1791,9 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>50</v>
+      <c r="E12" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机卡牌（光）</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -1274,8 +1809,9 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>50</v>
+      <c r="E13" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机卡牌（暗）</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -1291,8 +1827,9 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14">
-        <v>30</v>
+      <c r="E14" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(植物)</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -1308,8 +1845,9 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15">
-        <v>30</v>
+      <c r="E15" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(鱼)</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -1325,8 +1863,9 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16">
-        <v>30</v>
+      <c r="E16" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(矿石)</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -1342,8 +1881,9 @@
       <c r="D17">
         <v>2</v>
       </c>
-      <c r="E17">
-        <v>3</v>
+      <c r="E17" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>小型魔法药剂</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -1359,8 +1899,9 @@
       <c r="D18">
         <v>2</v>
       </c>
-      <c r="E18">
-        <v>5</v>
+      <c r="E18" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型魔法药剂</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -1376,8 +1917,9 @@
       <c r="D19">
         <v>2</v>
       </c>
-      <c r="E19">
-        <v>12</v>
+      <c r="E19" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型魔法药剂</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -1393,8 +1935,9 @@
       <c r="D20">
         <v>2</v>
       </c>
-      <c r="E20">
-        <v>3</v>
+      <c r="E20" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>小型恢复药剂</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -1410,8 +1953,9 @@
       <c r="D21">
         <v>2</v>
       </c>
-      <c r="E21">
-        <v>5</v>
+      <c r="E21" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型恢复药剂</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -1427,8 +1971,9 @@
       <c r="D22">
         <v>2</v>
       </c>
-      <c r="E22">
-        <v>12</v>
+      <c r="E22" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型恢复药剂</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -1444,8 +1989,9 @@
       <c r="D23">
         <v>2</v>
       </c>
-      <c r="E23">
-        <v>3</v>
+      <c r="E23" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>小型活力药剂</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -1461,8 +2007,9 @@
       <c r="D24">
         <v>2</v>
       </c>
-      <c r="E24">
-        <v>5</v>
+      <c r="E24" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型活力药剂</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -1478,8 +2025,9 @@
       <c r="D25">
         <v>2</v>
       </c>
-      <c r="E25">
-        <v>12</v>
+      <c r="E25" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型活力药剂</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -1495,8 +2043,9 @@
       <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26">
-        <v>5</v>
+      <c r="E26" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>药剂-命</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -1512,8 +2061,9 @@
       <c r="D27">
         <v>2</v>
       </c>
-      <c r="E27">
-        <v>5</v>
+      <c r="E27" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>体力药水</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -1529,8 +2079,9 @@
       <c r="D28">
         <v>2</v>
       </c>
-      <c r="E28">
-        <v>15</v>
+      <c r="E28" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>战斗药水</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -1546,8 +2097,9 @@
       <c r="D29">
         <v>2</v>
       </c>
-      <c r="E29">
-        <v>15</v>
+      <c r="E29" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>守护药水</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
@@ -1563,8 +2115,9 @@
       <c r="D30">
         <v>2</v>
       </c>
-      <c r="E30">
-        <v>15</v>
+      <c r="E30" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>法术药水</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -1580,8 +2133,9 @@
       <c r="D31">
         <v>2</v>
       </c>
-      <c r="E31">
-        <v>15</v>
+      <c r="E31" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>技巧药水</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
@@ -1597,8 +2151,9 @@
       <c r="D32">
         <v>2</v>
       </c>
-      <c r="E32">
-        <v>15</v>
+      <c r="E32" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>速度药水</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -1614,8 +2169,9 @@
       <c r="D33">
         <v>2</v>
       </c>
-      <c r="E33">
-        <v>15</v>
+      <c r="E33" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>幸运药水</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
@@ -1631,8 +2187,9 @@
       <c r="D34">
         <v>2</v>
       </c>
-      <c r="E34">
-        <v>15</v>
+      <c r="E34" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>体质药水</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -1648,8 +2205,9 @@
       <c r="D35">
         <v>2</v>
       </c>
-      <c r="E35">
-        <v>15</v>
+      <c r="E35" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>生存药水</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -1665,8 +2223,9 @@
       <c r="D36">
         <v>3</v>
       </c>
-      <c r="E36">
-        <v>7</v>
+      <c r="E36" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机幻兽卡</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -1682,8 +2241,9 @@
       <c r="D37">
         <v>3</v>
       </c>
-      <c r="E37">
-        <v>7</v>
+      <c r="E37" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机武器卡</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -1699,8 +2259,9 @@
       <c r="D38">
         <v>3</v>
       </c>
-      <c r="E38">
-        <v>7</v>
+      <c r="E38" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机魔法卡</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -1716,8 +2277,9 @@
       <c r="D39">
         <v>3</v>
       </c>
-      <c r="E39">
-        <v>3</v>
+      <c r="E39" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-艾尔</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
@@ -1733,8 +2295,9 @@
       <c r="D40">
         <v>3</v>
       </c>
-      <c r="E40">
-        <v>6</v>
+      <c r="E40" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-普尔</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -1750,8 +2313,9 @@
       <c r="D41">
         <v>3</v>
       </c>
-      <c r="E41">
-        <v>15</v>
+      <c r="E41" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-查姆</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
@@ -1767,8 +2331,9 @@
       <c r="D42">
         <v>3</v>
       </c>
-      <c r="E42">
-        <v>5</v>
+      <c r="E42" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>经验之书</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
@@ -1784,8 +2349,9 @@
       <c r="D43">
         <v>3</v>
       </c>
-      <c r="E43">
-        <v>30</v>
+      <c r="E43" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>能量之书</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
@@ -1801,8 +2367,9 @@
       <c r="D44">
         <v>3</v>
       </c>
-      <c r="E44">
-        <v>9</v>
+      <c r="E44" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>体力药水</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
@@ -1818,8 +2385,9 @@
       <c r="D45">
         <v>3</v>
       </c>
-      <c r="E45">
-        <v>9</v>
+      <c r="E45" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>体力药水</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
@@ -1835,8 +2403,9 @@
       <c r="D46">
         <v>3</v>
       </c>
-      <c r="E46">
-        <v>12</v>
+      <c r="E46" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>体力药水</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a a deckcard effect when can uplevel
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="GameShop" sheetId="1" r:id="rId1"/>
@@ -766,502 +766,826 @@
       <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="1">
+          <cell r="A1" t="str">
+            <v>序列</v>
+          </cell>
           <cell r="B1" t="str">
             <v>名字</v>
           </cell>
         </row>
         <row r="2">
+          <cell r="A2" t="str">
+            <v>int</v>
+          </cell>
           <cell r="B2" t="str">
             <v>string</v>
           </cell>
         </row>
         <row r="3">
+          <cell r="A3" t="str">
+            <v>Id</v>
+          </cell>
           <cell r="B3" t="str">
             <v>Name</v>
           </cell>
         </row>
         <row r="4">
+          <cell r="A4">
+            <v>22031001</v>
+          </cell>
           <cell r="B4" t="str">
             <v>新手礼包</v>
           </cell>
         </row>
         <row r="5">
+          <cell r="A5">
+            <v>22031002</v>
+          </cell>
           <cell r="B5" t="str">
-            <v>随机卡牌（无）</v>
+            <v>卡牌补给包（无）</v>
           </cell>
         </row>
         <row r="6">
+          <cell r="A6">
+            <v>22031003</v>
+          </cell>
           <cell r="B6" t="str">
-            <v>随机卡牌（水）</v>
+            <v>卡牌补给包（水）</v>
           </cell>
         </row>
         <row r="7">
+          <cell r="A7">
+            <v>22031004</v>
+          </cell>
           <cell r="B7" t="str">
-            <v>随机卡牌（风）</v>
+            <v>卡牌补给包（风）</v>
           </cell>
         </row>
         <row r="8">
+          <cell r="A8">
+            <v>22031005</v>
+          </cell>
           <cell r="B8" t="str">
-            <v>随机卡牌（地）</v>
+            <v>卡牌补给包（地）</v>
           </cell>
         </row>
         <row r="9">
+          <cell r="A9">
+            <v>22031006</v>
+          </cell>
           <cell r="B9" t="str">
-            <v>随机卡牌（火）</v>
+            <v>卡牌补给包（火）</v>
           </cell>
         </row>
         <row r="10">
+          <cell r="A10">
+            <v>22031007</v>
+          </cell>
           <cell r="B10" t="str">
-            <v>随机卡牌（光）</v>
+            <v>卡牌补给包（光）</v>
           </cell>
         </row>
         <row r="11">
+          <cell r="A11">
+            <v>22031008</v>
+          </cell>
           <cell r="B11" t="str">
-            <v>随机卡牌（暗）</v>
+            <v>卡牌补给包（暗）</v>
           </cell>
         </row>
         <row r="12">
+          <cell r="A12">
+            <v>22031011</v>
+          </cell>
           <cell r="B12" t="str">
+            <v>卡牌补给包（生物）</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>22031012</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>卡牌补给包（武器）</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>22031013</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>卡牌补给包（法术）</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>22031101</v>
+          </cell>
+          <cell r="B15" t="str">
             <v>资源袋(植物)</v>
           </cell>
         </row>
-        <row r="13">
-          <cell r="B13" t="str">
+        <row r="16">
+          <cell r="A16">
+            <v>22031102</v>
+          </cell>
+          <cell r="B16" t="str">
             <v>资源袋(鱼)</v>
           </cell>
         </row>
-        <row r="14">
-          <cell r="B14" t="str">
+        <row r="17">
+          <cell r="A17">
+            <v>22031103</v>
+          </cell>
+          <cell r="B17" t="str">
             <v>资源袋(矿石)</v>
           </cell>
         </row>
-        <row r="15">
-          <cell r="B15" t="str">
+        <row r="18">
+          <cell r="A18">
+            <v>22031201</v>
+          </cell>
+          <cell r="B18" t="str">
             <v>蓝色卡包</v>
           </cell>
         </row>
-        <row r="16">
-          <cell r="B16" t="str">
+        <row r="19">
+          <cell r="A19">
+            <v>22031202</v>
+          </cell>
+          <cell r="B19" t="str">
             <v>黄色卡包</v>
           </cell>
         </row>
-        <row r="17">
-          <cell r="B17" t="str">
+        <row r="20">
+          <cell r="A20">
+            <v>22031203</v>
+          </cell>
+          <cell r="B20" t="str">
             <v>红色卡包</v>
           </cell>
         </row>
-        <row r="18">
-          <cell r="B18" t="str">
+        <row r="21">
+          <cell r="A21">
+            <v>22032001</v>
+          </cell>
+          <cell r="B21" t="str">
             <v>木材补给车</v>
           </cell>
         </row>
-        <row r="19">
-          <cell r="B19" t="str">
+        <row r="22">
+          <cell r="A22">
+            <v>22032002</v>
+          </cell>
+          <cell r="B22" t="str">
             <v>矿石补给车</v>
           </cell>
         </row>
-        <row r="20">
-          <cell r="B20" t="str">
+        <row r="23">
+          <cell r="A23">
+            <v>22032003</v>
+          </cell>
+          <cell r="B23" t="str">
             <v>水银补给车</v>
           </cell>
         </row>
-        <row r="21">
-          <cell r="B21" t="str">
+        <row r="24">
+          <cell r="A24">
+            <v>22032004</v>
+          </cell>
+          <cell r="B24" t="str">
             <v>红宝石补给车</v>
           </cell>
         </row>
-        <row r="22">
-          <cell r="B22" t="str">
+        <row r="25">
+          <cell r="A25">
+            <v>22032005</v>
+          </cell>
+          <cell r="B25" t="str">
             <v>硫磺补给车</v>
           </cell>
         </row>
-        <row r="23">
-          <cell r="B23" t="str">
+        <row r="26">
+          <cell r="A26">
+            <v>22032006</v>
+          </cell>
+          <cell r="B26" t="str">
             <v>水晶补给车</v>
           </cell>
         </row>
-        <row r="24">
-          <cell r="B24" t="str">
+        <row r="27">
+          <cell r="A27">
+            <v>22032007</v>
+          </cell>
+          <cell r="B27" t="str">
             <v>初始资源包</v>
           </cell>
         </row>
-        <row r="25">
-          <cell r="B25" t="str">
+        <row r="28">
+          <cell r="A28">
+            <v>22032008</v>
+          </cell>
+          <cell r="B28" t="str">
             <v>金币</v>
           </cell>
         </row>
-        <row r="26">
-          <cell r="B26" t="str">
+        <row r="29">
+          <cell r="A29">
+            <v>22033001</v>
+          </cell>
+          <cell r="B29" t="str">
             <v>小型魔法药剂</v>
           </cell>
         </row>
-        <row r="27">
-          <cell r="B27" t="str">
+        <row r="30">
+          <cell r="A30">
+            <v>22033002</v>
+          </cell>
+          <cell r="B30" t="str">
             <v>中型魔法药剂</v>
           </cell>
         </row>
-        <row r="28">
-          <cell r="B28" t="str">
+        <row r="31">
+          <cell r="A31">
+            <v>22033003</v>
+          </cell>
+          <cell r="B31" t="str">
             <v>大型魔法药剂</v>
           </cell>
         </row>
-        <row r="29">
-          <cell r="B29" t="str">
+        <row r="32">
+          <cell r="A32">
+            <v>22033004</v>
+          </cell>
+          <cell r="B32" t="str">
             <v>小型恢复药剂</v>
           </cell>
         </row>
-        <row r="30">
-          <cell r="B30" t="str">
+        <row r="33">
+          <cell r="A33">
+            <v>22033005</v>
+          </cell>
+          <cell r="B33" t="str">
             <v>中型恢复药剂</v>
           </cell>
         </row>
-        <row r="31">
-          <cell r="B31" t="str">
+        <row r="34">
+          <cell r="A34">
+            <v>22033006</v>
+          </cell>
+          <cell r="B34" t="str">
             <v>大型恢复药剂</v>
           </cell>
         </row>
-        <row r="32">
-          <cell r="B32" t="str">
+        <row r="35">
+          <cell r="A35">
+            <v>22033007</v>
+          </cell>
+          <cell r="B35" t="str">
             <v>小型活力药剂</v>
           </cell>
         </row>
-        <row r="33">
-          <cell r="B33" t="str">
+        <row r="36">
+          <cell r="A36">
+            <v>22033008</v>
+          </cell>
+          <cell r="B36" t="str">
             <v>中型活力药剂</v>
           </cell>
         </row>
-        <row r="34">
-          <cell r="B34" t="str">
+        <row r="37">
+          <cell r="A37">
+            <v>22033009</v>
+          </cell>
+          <cell r="B37" t="str">
             <v>大型活力药剂</v>
           </cell>
         </row>
-        <row r="35">
-          <cell r="B35" t="str">
+        <row r="38">
+          <cell r="A38">
+            <v>22033013</v>
+          </cell>
+          <cell r="B38" t="str">
             <v>随机幻兽卡</v>
           </cell>
         </row>
-        <row r="36">
-          <cell r="B36" t="str">
+        <row r="39">
+          <cell r="A39">
+            <v>22033014</v>
+          </cell>
+          <cell r="B39" t="str">
             <v>随机武器卡</v>
           </cell>
         </row>
-        <row r="37">
-          <cell r="B37" t="str">
+        <row r="40">
+          <cell r="A40">
+            <v>22033015</v>
+          </cell>
+          <cell r="B40" t="str">
             <v>随机魔法卡</v>
           </cell>
         </row>
-        <row r="38">
-          <cell r="B38" t="str">
+        <row r="41">
+          <cell r="A41">
+            <v>22033016</v>
+          </cell>
+          <cell r="B41" t="str">
             <v>符文-查姆</v>
           </cell>
         </row>
-        <row r="39">
-          <cell r="B39" t="str">
+        <row r="42">
+          <cell r="A42">
+            <v>22033017</v>
+          </cell>
+          <cell r="B42" t="str">
             <v>符文-普尔</v>
           </cell>
         </row>
-        <row r="40">
-          <cell r="B40" t="str">
+        <row r="43">
+          <cell r="A43">
+            <v>22033018</v>
+          </cell>
+          <cell r="B43" t="str">
             <v>符文-艾尔</v>
           </cell>
         </row>
-        <row r="41">
-          <cell r="B41" t="str">
+        <row r="44">
+          <cell r="A44">
+            <v>22033030</v>
+          </cell>
+          <cell r="B44" t="str">
             <v>小型药剂-命</v>
           </cell>
         </row>
-        <row r="42">
-          <cell r="B42" t="str">
+        <row r="45">
+          <cell r="A45">
+            <v>22033031</v>
+          </cell>
+          <cell r="B45" t="str">
             <v>药剂-命</v>
           </cell>
         </row>
-        <row r="43">
-          <cell r="B43" t="str">
+        <row r="46">
+          <cell r="A46">
+            <v>22033032</v>
+          </cell>
+          <cell r="B46" t="str">
             <v>大型药剂-命</v>
           </cell>
         </row>
-        <row r="44">
-          <cell r="B44" t="str">
+        <row r="47">
+          <cell r="A47">
+            <v>22034001</v>
+          </cell>
+          <cell r="B47" t="str">
             <v>经验之书</v>
           </cell>
         </row>
-        <row r="45">
-          <cell r="B45" t="str">
+        <row r="48">
+          <cell r="A48">
+            <v>22034002</v>
+          </cell>
+          <cell r="B48" t="str">
             <v>能量之书</v>
           </cell>
         </row>
-        <row r="46">
-          <cell r="B46" t="str">
+        <row r="49">
+          <cell r="A49">
+            <v>22034003</v>
+          </cell>
+          <cell r="B49" t="str">
             <v>战斗药水</v>
           </cell>
         </row>
-        <row r="47">
-          <cell r="B47" t="str">
+        <row r="50">
+          <cell r="A50">
+            <v>22034004</v>
+          </cell>
+          <cell r="B50" t="str">
             <v>守护药水</v>
           </cell>
         </row>
-        <row r="48">
-          <cell r="B48" t="str">
+        <row r="51">
+          <cell r="A51">
+            <v>22034005</v>
+          </cell>
+          <cell r="B51" t="str">
             <v>法术药水</v>
           </cell>
         </row>
-        <row r="49">
-          <cell r="B49" t="str">
+        <row r="52">
+          <cell r="A52">
+            <v>22034006</v>
+          </cell>
+          <cell r="B52" t="str">
             <v>技巧药水</v>
           </cell>
         </row>
-        <row r="50">
-          <cell r="B50" t="str">
+        <row r="53">
+          <cell r="A53">
+            <v>22034007</v>
+          </cell>
+          <cell r="B53" t="str">
             <v>速度药水</v>
           </cell>
         </row>
-        <row r="51">
-          <cell r="B51" t="str">
+        <row r="54">
+          <cell r="A54">
+            <v>22034008</v>
+          </cell>
+          <cell r="B54" t="str">
             <v>幸运药水</v>
           </cell>
         </row>
-        <row r="52">
-          <cell r="B52" t="str">
+        <row r="55">
+          <cell r="A55">
+            <v>22034009</v>
+          </cell>
+          <cell r="B55" t="str">
             <v>体质药水</v>
           </cell>
         </row>
-        <row r="53">
-          <cell r="B53" t="str">
+        <row r="56">
+          <cell r="A56">
+            <v>22034010</v>
+          </cell>
+          <cell r="B56" t="str">
             <v>生存药水</v>
           </cell>
         </row>
-        <row r="54">
-          <cell r="B54" t="str">
+        <row r="57">
+          <cell r="A57">
+            <v>22034011</v>
+          </cell>
+          <cell r="B57" t="str">
             <v>体力药水</v>
           </cell>
         </row>
-        <row r="55">
-          <cell r="B55" t="str">
+        <row r="58">
+          <cell r="A58">
+            <v>22035001</v>
+          </cell>
+          <cell r="B58" t="str">
             <v>猛兽卡片</v>
           </cell>
         </row>
-        <row r="56">
-          <cell r="B56" t="str">
+        <row r="59">
+          <cell r="A59">
+            <v>22035002</v>
+          </cell>
+          <cell r="B59" t="str">
             <v>战斧卡片</v>
           </cell>
         </row>
-        <row r="57">
-          <cell r="B57" t="str">
+        <row r="60">
+          <cell r="A60">
+            <v>22035003</v>
+          </cell>
+          <cell r="B60" t="str">
             <v>火焰卡片</v>
           </cell>
         </row>
-        <row r="58">
-          <cell r="B58" t="str">
+        <row r="61">
+          <cell r="A61">
+            <v>22036101</v>
+          </cell>
+          <cell r="B61" t="str">
             <v>名片-塞尼斯</v>
           </cell>
         </row>
-        <row r="59">
-          <cell r="B59" t="str">
+        <row r="62">
+          <cell r="A62">
+            <v>22036102</v>
+          </cell>
+          <cell r="B62" t="str">
             <v>名片-塞巴斯恰恩</v>
           </cell>
         </row>
-        <row r="60">
-          <cell r="B60" t="str">
+        <row r="63">
+          <cell r="A63">
+            <v>22036103</v>
+          </cell>
+          <cell r="B63" t="str">
             <v>名片-科迪</v>
           </cell>
         </row>
-        <row r="61">
-          <cell r="B61" t="str">
+        <row r="64">
+          <cell r="A64">
+            <v>22036104</v>
+          </cell>
+          <cell r="B64" t="str">
             <v>名片-威阿伊丁</v>
           </cell>
         </row>
-        <row r="62">
-          <cell r="B62" t="str">
+        <row r="65">
+          <cell r="A65">
+            <v>22036105</v>
+          </cell>
+          <cell r="B65" t="str">
             <v>名片-奥莱伊李</v>
           </cell>
         </row>
-        <row r="63">
-          <cell r="B63" t="str">
+        <row r="66">
+          <cell r="A66">
+            <v>22036106</v>
+          </cell>
+          <cell r="B66" t="str">
             <v>名片-米兰达</v>
           </cell>
         </row>
-        <row r="64">
-          <cell r="B64" t="str">
+        <row r="67">
+          <cell r="A67">
+            <v>22036107</v>
+          </cell>
+          <cell r="B67" t="str">
             <v>名片-盖露贝尔</v>
           </cell>
         </row>
-        <row r="65">
-          <cell r="B65" t="str">
+        <row r="68">
+          <cell r="A68">
+            <v>22036108</v>
+          </cell>
+          <cell r="B68" t="str">
             <v>名片-贝露凯伊鲁</v>
           </cell>
         </row>
-        <row r="66">
-          <cell r="B66" t="str">
+        <row r="69">
+          <cell r="A69">
+            <v>22036109</v>
+          </cell>
+          <cell r="B69" t="str">
             <v>名片-雷洛比克</v>
           </cell>
         </row>
-        <row r="67">
-          <cell r="B67" t="str">
+        <row r="70">
+          <cell r="A70">
+            <v>22036110</v>
+          </cell>
+          <cell r="B70" t="str">
             <v>名片-巴鲁迪亚斯</v>
           </cell>
         </row>
-        <row r="68">
-          <cell r="B68" t="str">
+        <row r="71">
+          <cell r="A71">
+            <v>22036201</v>
+          </cell>
+          <cell r="B71" t="str">
             <v>名片-武藤游戏</v>
           </cell>
         </row>
-        <row r="69">
-          <cell r="B69" t="str">
+        <row r="72">
+          <cell r="A72">
+            <v>22036202</v>
+          </cell>
+          <cell r="B72" t="str">
             <v>名片-城之内</v>
           </cell>
         </row>
-        <row r="70">
-          <cell r="B70" t="str">
+        <row r="73">
+          <cell r="A73">
+            <v>22036203</v>
+          </cell>
+          <cell r="B73" t="str">
             <v>名片-海马懒人</v>
           </cell>
         </row>
-        <row r="71">
-          <cell r="B71" t="str">
+        <row r="74">
+          <cell r="A74">
+            <v>22036301</v>
+          </cell>
+          <cell r="B74" t="str">
             <v>名片-内芙妮</v>
           </cell>
         </row>
-        <row r="72">
-          <cell r="B72" t="str">
+        <row r="75">
+          <cell r="A75">
+            <v>22036302</v>
+          </cell>
+          <cell r="B75" t="str">
             <v>名片-塔妮丝</v>
           </cell>
         </row>
-        <row r="73">
-          <cell r="B73" t="str">
+        <row r="76">
+          <cell r="A76">
+            <v>22036303</v>
+          </cell>
+          <cell r="B76" t="str">
             <v>名片-卢卡</v>
           </cell>
         </row>
-        <row r="74">
-          <cell r="B74" t="str">
+        <row r="77">
+          <cell r="A77">
+            <v>22036304</v>
+          </cell>
+          <cell r="B77" t="str">
             <v>名片-艾斯特尔</v>
           </cell>
         </row>
-        <row r="75">
-          <cell r="B75" t="str">
+        <row r="78">
+          <cell r="A78">
+            <v>22036305</v>
+          </cell>
+          <cell r="B78" t="str">
             <v>名片-萨恩</v>
           </cell>
         </row>
-        <row r="76">
-          <cell r="B76" t="str">
+        <row r="79">
+          <cell r="A79">
+            <v>22036306</v>
+          </cell>
+          <cell r="B79" t="str">
             <v>名片-玛莎</v>
           </cell>
         </row>
-        <row r="77">
-          <cell r="B77" t="str">
+        <row r="80">
+          <cell r="A80">
+            <v>22036307</v>
+          </cell>
+          <cell r="B80" t="str">
             <v>名片-阿特罗姆</v>
           </cell>
         </row>
-        <row r="78">
-          <cell r="B78" t="str">
+        <row r="81">
+          <cell r="A81">
+            <v>22036308</v>
+          </cell>
+          <cell r="B81" t="str">
             <v>名片-泽诺</v>
           </cell>
         </row>
-        <row r="79">
-          <cell r="B79" t="str">
+        <row r="82">
+          <cell r="A82">
+            <v>22036309</v>
+          </cell>
+          <cell r="B82" t="str">
             <v>名片-拉凯尔</v>
           </cell>
         </row>
-        <row r="80">
-          <cell r="B80" t="str">
+        <row r="83">
+          <cell r="A83">
+            <v>22036310</v>
+          </cell>
+          <cell r="B83" t="str">
             <v>名片-纳尔萨斯</v>
           </cell>
         </row>
-        <row r="81">
-          <cell r="B81" t="str">
+        <row r="84">
+          <cell r="A84">
+            <v>22036311</v>
+          </cell>
+          <cell r="B84" t="str">
             <v>名片-纳隆</v>
           </cell>
         </row>
-        <row r="82">
-          <cell r="B82" t="str">
+        <row r="85">
+          <cell r="A85">
+            <v>22036312</v>
+          </cell>
+          <cell r="B85" t="str">
             <v>名片-维加</v>
           </cell>
         </row>
-        <row r="83">
-          <cell r="B83" t="str">
+        <row r="86">
+          <cell r="A86">
+            <v>22036401</v>
+          </cell>
+          <cell r="B86" t="str">
             <v>名片-诺德</v>
           </cell>
         </row>
-        <row r="84">
-          <cell r="B84" t="str">
+        <row r="87">
+          <cell r="A87">
+            <v>22036402</v>
+          </cell>
+          <cell r="B87" t="str">
             <v>名片-那那美</v>
           </cell>
         </row>
-        <row r="85">
-          <cell r="B85" t="str">
+        <row r="88">
+          <cell r="A88">
+            <v>22036403</v>
+          </cell>
+          <cell r="B88" t="str">
             <v>名片-弗兰克</v>
           </cell>
         </row>
-        <row r="86">
-          <cell r="B86" t="str">
+        <row r="89">
+          <cell r="A89">
+            <v>22036404</v>
+          </cell>
+          <cell r="B89" t="str">
             <v>名片-维克托</v>
           </cell>
         </row>
-        <row r="87">
-          <cell r="B87" t="str">
+        <row r="90">
+          <cell r="A90">
+            <v>22036405</v>
+          </cell>
+          <cell r="B90" t="str">
             <v>名片-洛克</v>
           </cell>
         </row>
-        <row r="88">
-          <cell r="B88" t="str">
+        <row r="91">
+          <cell r="A91">
+            <v>22036406</v>
+          </cell>
+          <cell r="B91" t="str">
             <v>名片-谢拉</v>
           </cell>
         </row>
-        <row r="89">
-          <cell r="B89" t="str">
+        <row r="92">
+          <cell r="A92">
+            <v>22036407</v>
+          </cell>
+          <cell r="B92" t="str">
             <v>名片-克莱布</v>
           </cell>
         </row>
-        <row r="90">
-          <cell r="B90" t="str">
+        <row r="93">
+          <cell r="A93">
+            <v>22036408</v>
+          </cell>
+          <cell r="B93" t="str">
             <v>名片-蔡</v>
           </cell>
         </row>
-        <row r="91">
-          <cell r="B91" t="str">
+        <row r="94">
+          <cell r="A94">
+            <v>22036501</v>
+          </cell>
+          <cell r="B94" t="str">
             <v>名片-约修亚</v>
           </cell>
         </row>
-        <row r="92">
-          <cell r="B92" t="str">
+        <row r="95">
+          <cell r="A95">
+            <v>22036502</v>
+          </cell>
+          <cell r="B95" t="str">
             <v>名片-艾斯蒂尔</v>
           </cell>
         </row>
-        <row r="93">
-          <cell r="B93" t="str">
+        <row r="96">
+          <cell r="A96">
+            <v>22037001</v>
+          </cell>
+          <cell r="B96" t="str">
             <v>种子-豌豆</v>
           </cell>
         </row>
-        <row r="94">
-          <cell r="B94" t="str">
+        <row r="97">
+          <cell r="A97">
+            <v>22037002</v>
+          </cell>
+          <cell r="B97" t="str">
             <v>种子-玉米</v>
           </cell>
         </row>
-        <row r="95">
-          <cell r="B95" t="str">
+        <row r="98">
+          <cell r="A98">
+            <v>22037003</v>
+          </cell>
+          <cell r="B98" t="str">
             <v>种子-苹果</v>
           </cell>
         </row>
-        <row r="96">
-          <cell r="B96" t="str">
+        <row r="99">
+          <cell r="A99">
+            <v>22037004</v>
+          </cell>
+          <cell r="B99" t="str">
             <v>种子-蓝莓</v>
           </cell>
         </row>
-        <row r="97">
-          <cell r="B97" t="str">
+        <row r="100">
+          <cell r="A100">
+            <v>22037101</v>
+          </cell>
+          <cell r="B100" t="str">
             <v>作物-豌豆</v>
           </cell>
         </row>
-        <row r="98">
-          <cell r="B98" t="str">
+        <row r="101">
+          <cell r="A101">
+            <v>22037102</v>
+          </cell>
+          <cell r="B101" t="str">
             <v>作物-豌豆</v>
           </cell>
         </row>
-        <row r="99">
-          <cell r="B99" t="str">
+        <row r="102">
+          <cell r="A102">
+            <v>22037103</v>
+          </cell>
+          <cell r="B102" t="str">
             <v>作物-苹果</v>
           </cell>
         </row>
-        <row r="100">
-          <cell r="B100" t="str">
+        <row r="103">
+          <cell r="A103">
+            <v>22037104</v>
+          </cell>
+          <cell r="B103" t="str">
             <v>作物-蓝莓</v>
           </cell>
         </row>
@@ -1272,8 +1596,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E46" totalsRowShown="0">
-  <autoFilter ref="A1:E46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E43" totalsRowShown="0">
+  <autoFilter ref="A1:E43"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="ItemId"/>
@@ -1572,18 +1896,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1600,7 +1924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +1941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1634,7 +1958,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>15000001</v>
       </c>
@@ -1652,7 +1976,7 @@
         <v>猛兽卡片</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15000002</v>
       </c>
@@ -1670,7 +1994,7 @@
         <v>战斧卡片</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15000003</v>
       </c>
@@ -1688,7 +2012,7 @@
         <v>火焰卡片</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15000004</v>
       </c>
@@ -1703,10 +2027,10 @@
       </c>
       <c r="E7" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机卡牌（无）</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+        <v>卡牌补给包（无）</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15000005</v>
       </c>
@@ -1721,10 +2045,10 @@
       </c>
       <c r="E8" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机卡牌（水）</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+        <v>卡牌补给包（水）</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>15000006</v>
       </c>
@@ -1739,10 +2063,10 @@
       </c>
       <c r="E9" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机卡牌（风）</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+        <v>卡牌补给包（风）</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>15000007</v>
       </c>
@@ -1757,10 +2081,10 @@
       </c>
       <c r="E10" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机卡牌（地）</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+        <v>卡牌补给包（地）</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15000008</v>
       </c>
@@ -1775,10 +2099,10 @@
       </c>
       <c r="E11" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机卡牌（火）</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+        <v>卡牌补给包（火）</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>15000009</v>
       </c>
@@ -1793,10 +2117,10 @@
       </c>
       <c r="E12" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机卡牌（光）</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+        <v>卡牌补给包（光）</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15000010</v>
       </c>
@@ -1811,10 +2135,10 @@
       </c>
       <c r="E13" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机卡牌（暗）</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+        <v>卡牌补给包（暗）</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15000011</v>
       </c>
@@ -1832,7 +2156,7 @@
         <v>资源袋(植物)</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15000012</v>
       </c>
@@ -1850,7 +2174,7 @@
         <v>资源袋(鱼)</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15000013</v>
       </c>
@@ -1868,7 +2192,7 @@
         <v>资源袋(矿石)</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15000014</v>
       </c>
@@ -1886,7 +2210,7 @@
         <v>小型魔法药剂</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15000015</v>
       </c>
@@ -1904,7 +2228,7 @@
         <v>中型魔法药剂</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15000016</v>
       </c>
@@ -1922,7 +2246,7 @@
         <v>大型魔法药剂</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15000017</v>
       </c>
@@ -1940,7 +2264,7 @@
         <v>小型恢复药剂</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15000018</v>
       </c>
@@ -1958,7 +2282,7 @@
         <v>中型恢复药剂</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15000019</v>
       </c>
@@ -1976,7 +2300,7 @@
         <v>大型恢复药剂</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15000020</v>
       </c>
@@ -1994,7 +2318,7 @@
         <v>小型活力药剂</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15000021</v>
       </c>
@@ -2012,7 +2336,7 @@
         <v>中型活力药剂</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>15000022</v>
       </c>
@@ -2030,7 +2354,7 @@
         <v>大型活力药剂</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>15000023</v>
       </c>
@@ -2048,7 +2372,7 @@
         <v>药剂-命</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15000024</v>
       </c>
@@ -2066,7 +2390,7 @@
         <v>体力药水</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>15000025</v>
       </c>
@@ -2084,7 +2408,7 @@
         <v>战斗药水</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15000026</v>
       </c>
@@ -2102,7 +2426,7 @@
         <v>守护药水</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>15000027</v>
       </c>
@@ -2120,7 +2444,7 @@
         <v>法术药水</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>15000028</v>
       </c>
@@ -2138,7 +2462,7 @@
         <v>技巧药水</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>15000029</v>
       </c>
@@ -2156,7 +2480,7 @@
         <v>速度药水</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>15000030</v>
       </c>
@@ -2174,7 +2498,7 @@
         <v>幸运药水</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>15000031</v>
       </c>
@@ -2192,7 +2516,7 @@
         <v>体质药水</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>15000032</v>
       </c>
@@ -2210,7 +2534,7 @@
         <v>生存药水</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15000033</v>
       </c>
@@ -2228,7 +2552,7 @@
         <v>随机幻兽卡</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>15000034</v>
       </c>
@@ -2246,7 +2570,7 @@
         <v>随机武器卡</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>15000035</v>
       </c>
@@ -2264,7 +2588,7 @@
         <v>随机魔法卡</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>15000036</v>
       </c>
@@ -2282,7 +2606,7 @@
         <v>符文-艾尔</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>15000037</v>
       </c>
@@ -2300,7 +2624,7 @@
         <v>符文-普尔</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>15000038</v>
       </c>
@@ -2318,7 +2642,7 @@
         <v>符文-查姆</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>15000039</v>
       </c>
@@ -2336,7 +2660,7 @@
         <v>经验之书</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>15000040</v>
       </c>
@@ -2352,60 +2676,6 @@
       <c r="E43" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>能量之书</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44">
-        <v>15000041</v>
-      </c>
-      <c r="B44">
-        <v>22034012</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>3</v>
-      </c>
-      <c r="E44" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>体力药水</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45">
-        <v>15000042</v>
-      </c>
-      <c r="B45">
-        <v>22034013</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>3</v>
-      </c>
-      <c r="E45" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>体力药水</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46">
-        <v>15000043</v>
-      </c>
-      <c r="B46">
-        <v>22034014</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>3</v>
-      </c>
-      <c r="E46" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>体力药水</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#87 remake the potion and sale in gameshop
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -1154,7 +1154,7 @@
             <v>22034003</v>
           </cell>
           <cell r="B49" t="str">
-            <v>战斗药水</v>
+            <v>攻速药水</v>
           </cell>
         </row>
         <row r="50">
@@ -1202,7 +1202,7 @@
             <v>22034009</v>
           </cell>
           <cell r="B55" t="str">
-            <v>体质药水</v>
+            <v>暴击药水</v>
           </cell>
         </row>
         <row r="56">
@@ -1596,8 +1596,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E43" totalsRowShown="0">
-  <autoFilter ref="A1:E43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E42" totalsRowShown="0">
+  <autoFilter ref="A1:E42"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="ItemId"/>
@@ -1896,10 +1896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="E28" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>战斗药水</v>
+        <v>攻速药水</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2513,33 +2513,33 @@
       </c>
       <c r="E34" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>体质药水</v>
+        <v>暴击药水</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>15000032</v>
+        <v>15000033</v>
       </c>
       <c r="B35">
-        <v>22034010</v>
+        <v>22033013</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E35" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>生存药水</v>
+        <v>随机幻兽卡</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>15000033</v>
+        <v>15000034</v>
       </c>
       <c r="B36">
-        <v>22033013</v>
+        <v>22033014</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2549,15 +2549,15 @@
       </c>
       <c r="E36" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机幻兽卡</v>
+        <v>随机武器卡</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>15000034</v>
+        <v>15000035</v>
       </c>
       <c r="B37">
-        <v>22033014</v>
+        <v>22033015</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2567,15 +2567,15 @@
       </c>
       <c r="E37" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机武器卡</v>
+        <v>随机魔法卡</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>15000035</v>
+        <v>15000036</v>
       </c>
       <c r="B38">
-        <v>22033015</v>
+        <v>22033018</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2585,15 +2585,15 @@
       </c>
       <c r="E38" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机魔法卡</v>
+        <v>符文-艾尔</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>15000036</v>
+        <v>15000037</v>
       </c>
       <c r="B39">
-        <v>22033018</v>
+        <v>22033017</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2603,15 +2603,15 @@
       </c>
       <c r="E39" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-艾尔</v>
+        <v>符文-普尔</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>15000037</v>
+        <v>15000038</v>
       </c>
       <c r="B40">
-        <v>22033017</v>
+        <v>22033016</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2621,15 +2621,15 @@
       </c>
       <c r="E40" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-普尔</v>
+        <v>符文-查姆</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>15000038</v>
+        <v>15000039</v>
       </c>
       <c r="B41">
-        <v>22033016</v>
+        <v>22034001</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2639,15 +2639,15 @@
       </c>
       <c r="E41" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-查姆</v>
+        <v>经验之书</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>15000039</v>
+        <v>15000040</v>
       </c>
       <c r="B42">
-        <v>22034001</v>
+        <v>22034002</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2656,24 +2656,6 @@
         <v>3</v>
       </c>
       <c r="E42" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>经验之书</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>15000040</v>
-      </c>
-      <c r="B43">
-        <v>22034002</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <v>3</v>
-      </c>
-      <c r="E43" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>能量之书</v>
       </c>

</xml_diff>

<commit_message>
#87 remend all the recover potion item
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -441,7 +441,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -556,6 +556,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -685,7 +716,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -693,6 +724,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1018,7 +1058,7 @@
             <v>22033004</v>
           </cell>
           <cell r="B32" t="str">
-            <v>小型恢复药剂</v>
+            <v>小型活力药剂</v>
           </cell>
         </row>
         <row r="33">
@@ -1026,7 +1066,7 @@
             <v>22033005</v>
           </cell>
           <cell r="B33" t="str">
-            <v>中型恢复药剂</v>
+            <v>中型活力药剂</v>
           </cell>
         </row>
         <row r="34">
@@ -1034,7 +1074,7 @@
             <v>22033006</v>
           </cell>
           <cell r="B34" t="str">
-            <v>大型恢复药剂</v>
+            <v>大型活力药剂</v>
           </cell>
         </row>
         <row r="35">
@@ -1042,7 +1082,7 @@
             <v>22033007</v>
           </cell>
           <cell r="B35" t="str">
-            <v>小型活力药剂</v>
+            <v>小型体力药剂</v>
           </cell>
         </row>
         <row r="36">
@@ -1050,7 +1090,7 @@
             <v>22033008</v>
           </cell>
           <cell r="B36" t="str">
-            <v>中型活力药剂</v>
+            <v>中型体力药剂</v>
           </cell>
         </row>
         <row r="37">
@@ -1058,7 +1098,7 @@
             <v>22033009</v>
           </cell>
           <cell r="B37" t="str">
-            <v>大型活力药剂</v>
+            <v>大型体力药剂</v>
           </cell>
         </row>
         <row r="38">
@@ -1898,12 +1938,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2193,57 +2234,57 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>15000014</v>
       </c>
-      <c r="B17">
-        <v>22033001</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
+      <c r="B17" s="4">
+        <v>22033004</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4">
         <v>2</v>
       </c>
-      <c r="E17" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>小型魔法药剂</v>
+      <c r="E17" s="5" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>小型活力药剂</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>15000015</v>
       </c>
-      <c r="B18">
-        <v>22033002</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
+      <c r="B18" s="4">
+        <v>22033005</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4">
         <v>2</v>
       </c>
-      <c r="E18" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>中型魔法药剂</v>
+      <c r="E18" s="5" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型活力药剂</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>15000016</v>
       </c>
-      <c r="B19">
-        <v>22033003</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
+      <c r="B19" s="4">
+        <v>22033006</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
         <v>2</v>
       </c>
-      <c r="E19" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型魔法药剂</v>
+      <c r="E19" s="5" t="str">
+        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型活力药剂</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2251,7 +2292,7 @@
         <v>15000017</v>
       </c>
       <c r="B20">
-        <v>22033004</v>
+        <v>22033001</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2261,7 +2302,7 @@
       </c>
       <c r="E20" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>小型恢复药剂</v>
+        <v>小型魔法药剂</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2269,7 +2310,7 @@
         <v>15000018</v>
       </c>
       <c r="B21">
-        <v>22033005</v>
+        <v>22033002</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2279,7 +2320,7 @@
       </c>
       <c r="E21" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>中型恢复药剂</v>
+        <v>中型魔法药剂</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2287,7 +2328,7 @@
         <v>15000019</v>
       </c>
       <c r="B22">
-        <v>22033006</v>
+        <v>22033003</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2297,7 +2338,7 @@
       </c>
       <c r="E22" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型恢复药剂</v>
+        <v>大型魔法药剂</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2315,7 +2356,7 @@
       </c>
       <c r="E23" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>小型活力药剂</v>
+        <v>小型体力药剂</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2333,7 +2374,7 @@
       </c>
       <c r="E24" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>中型活力药剂</v>
+        <v>中型体力药剂</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2351,7 +2392,7 @@
       </c>
       <c r="E25" t="str">
         <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型活力药剂</v>
+        <v>大型体力药剂</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
#87 finish the shopitem mend-hammer
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,7 +12,7 @@
     <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
-    <sheet name="GameShop" sheetId="1" r:id="rId1"/>
+    <sheet name="GameShop" sheetId="2" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -24,26 +24,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>装备/道具id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>货架id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -51,30 +31,40 @@
   </si>
   <si>
     <t>Id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>ItemId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
   </si>
   <si>
     <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列</t>
+  </si>
+  <si>
+    <t>装备/道具id</t>
+  </si>
+  <si>
+    <t>类型</t>
+  </si>
+  <si>
+    <t>货架id</t>
   </si>
   <si>
     <t>道具名</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,24 +225,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -436,12 +408,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -557,26 +529,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="4"/>
@@ -716,23 +668,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -780,7 +723,38 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1636,14 +1610,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E42" totalsRowShown="0">
-  <autoFilter ref="A1:E42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:E40" totalsRowShown="0">
+  <autoFilter ref="A3:E40"/>
+  <sortState ref="A4:E42">
+    <sortCondition ref="A3:A42"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="ItemId"/>
     <tableColumn id="3" name="Type"/>
     <tableColumn id="4" name="Shelf"/>
-    <tableColumn id="5" name="Name"/>
+    <tableColumn id="5" name="Name" dataDxfId="0">
+      <calculatedColumnFormula>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1936,67 +1915,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2012,8 +1990,8 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E4" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>猛兽卡片</v>
       </c>
     </row>
@@ -2030,8 +2008,8 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E5" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>战斧卡片</v>
       </c>
     </row>
@@ -2048,8 +2026,8 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E6" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>火焰卡片</v>
       </c>
     </row>
@@ -2066,8 +2044,8 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E7" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（无）</v>
       </c>
     </row>
@@ -2084,8 +2062,8 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E8" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（水）</v>
       </c>
     </row>
@@ -2102,8 +2080,8 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E9" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（风）</v>
       </c>
     </row>
@@ -2120,8 +2098,8 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E10" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（地）</v>
       </c>
     </row>
@@ -2138,8 +2116,8 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E11" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（火）</v>
       </c>
     </row>
@@ -2156,8 +2134,8 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E12" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（光）</v>
       </c>
     </row>
@@ -2174,8 +2152,8 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E13" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（暗）</v>
       </c>
     </row>
@@ -2192,8 +2170,8 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E14" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(植物)</v>
       </c>
     </row>
@@ -2210,8 +2188,8 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E15" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(鱼)</v>
       </c>
     </row>
@@ -2228,63 +2206,63 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+      <c r="E16" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(矿石)</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17">
         <v>15000014</v>
       </c>
-      <c r="B17" s="4">
-        <v>22033004</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="B17">
+        <v>22033013</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="E17" s="5" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>小型活力药剂</v>
+      <c r="E17" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机幻兽卡</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18">
         <v>15000015</v>
       </c>
-      <c r="B18" s="4">
-        <v>22033005</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="B18">
+        <v>22033014</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
         <v>2</v>
       </c>
-      <c r="E18" s="5" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>中型活力药剂</v>
+      <c r="E18" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机武器卡</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19">
         <v>15000016</v>
       </c>
-      <c r="B19" s="4">
-        <v>22033006</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4">
+      <c r="B19">
+        <v>22033015</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
         <v>2</v>
       </c>
-      <c r="E19" s="5" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型活力药剂</v>
+      <c r="E19" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机魔法卡</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2292,7 +2270,7 @@
         <v>15000017</v>
       </c>
       <c r="B20">
-        <v>22033001</v>
+        <v>22033018</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2300,9 +2278,9 @@
       <c r="D20">
         <v>2</v>
       </c>
-      <c r="E20" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>小型魔法药剂</v>
+      <c r="E20" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-艾尔</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2310,7 +2288,7 @@
         <v>15000018</v>
       </c>
       <c r="B21">
-        <v>22033002</v>
+        <v>22033017</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2318,9 +2296,9 @@
       <c r="D21">
         <v>2</v>
       </c>
-      <c r="E21" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>中型魔法药剂</v>
+      <c r="E21" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-普尔</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2328,7 +2306,7 @@
         <v>15000019</v>
       </c>
       <c r="B22">
-        <v>22033003</v>
+        <v>22033016</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2336,17 +2314,17 @@
       <c r="D22">
         <v>2</v>
       </c>
-      <c r="E22" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型魔法药剂</v>
+      <c r="E22" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-查姆</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>15000020</v>
+        <v>15000021</v>
       </c>
       <c r="B23">
-        <v>22033007</v>
+        <v>22033005</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2354,17 +2332,17 @@
       <c r="D23">
         <v>2</v>
       </c>
-      <c r="E23" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>小型体力药剂</v>
+      <c r="E23" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型活力药剂</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>15000021</v>
+        <v>15000022</v>
       </c>
       <c r="B24">
-        <v>22033008</v>
+        <v>22033006</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2372,17 +2350,17 @@
       <c r="D24">
         <v>2</v>
       </c>
-      <c r="E24" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>中型体力药剂</v>
+      <c r="E24" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型活力药剂</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>15000022</v>
+        <v>15000024</v>
       </c>
       <c r="B25">
-        <v>22033009</v>
+        <v>22033002</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2390,17 +2368,17 @@
       <c r="D25">
         <v>2</v>
       </c>
-      <c r="E25" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型体力药剂</v>
+      <c r="E25" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型魔法药剂</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>15000023</v>
+        <v>15000025</v>
       </c>
       <c r="B26">
-        <v>22033031</v>
+        <v>22033003</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2408,17 +2386,17 @@
       <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>药剂-命</v>
+      <c r="E26" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型魔法药剂</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>15000024</v>
+        <v>15000026</v>
       </c>
       <c r="B27">
-        <v>22034011</v>
+        <v>22033008</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2426,17 +2404,17 @@
       <c r="D27">
         <v>2</v>
       </c>
-      <c r="E27" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>体力药水</v>
+      <c r="E27" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型体力药剂</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>15000025</v>
+        <v>15000027</v>
       </c>
       <c r="B28">
-        <v>22034003</v>
+        <v>22033009</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2444,17 +2422,17 @@
       <c r="D28">
         <v>2</v>
       </c>
-      <c r="E28" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>攻速药水</v>
+      <c r="E28" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型体力药剂</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>15000026</v>
+        <v>15000028</v>
       </c>
       <c r="B29">
-        <v>22034004</v>
+        <v>22033031</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2462,17 +2440,17 @@
       <c r="D29">
         <v>2</v>
       </c>
-      <c r="E29" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>守护药水</v>
+      <c r="E29" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>药剂-命</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>15000027</v>
+        <v>15000029</v>
       </c>
       <c r="B30">
-        <v>22034005</v>
+        <v>22033032</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2480,17 +2458,17 @@
       <c r="D30">
         <v>2</v>
       </c>
-      <c r="E30" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>法术药水</v>
+      <c r="E30" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型药剂-命</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>15000028</v>
+        <v>15000030</v>
       </c>
       <c r="B31">
-        <v>22034006</v>
+        <v>22034003</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2498,17 +2476,17 @@
       <c r="D31">
         <v>2</v>
       </c>
-      <c r="E31" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>技巧药水</v>
+      <c r="E31" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>攻速药水</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>15000029</v>
+        <v>15000031</v>
       </c>
       <c r="B32">
-        <v>22034007</v>
+        <v>22034004</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2516,17 +2494,17 @@
       <c r="D32">
         <v>2</v>
       </c>
-      <c r="E32" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>速度药水</v>
+      <c r="E32" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>守护药水</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>15000030</v>
+        <v>15000032</v>
       </c>
       <c r="B33">
-        <v>22034008</v>
+        <v>22034005</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2534,17 +2512,17 @@
       <c r="D33">
         <v>2</v>
       </c>
-      <c r="E33" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>幸运药水</v>
+      <c r="E33" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>法术药水</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>15000031</v>
+        <v>15000033</v>
       </c>
       <c r="B34">
-        <v>22034009</v>
+        <v>22034006</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2552,71 +2530,71 @@
       <c r="D34">
         <v>2</v>
       </c>
-      <c r="E34" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>暴击药水</v>
+      <c r="E34" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>技巧药水</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>15000033</v>
+        <v>15000034</v>
       </c>
       <c r="B35">
-        <v>22033013</v>
+        <v>22034007</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>3</v>
-      </c>
-      <c r="E35" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机幻兽卡</v>
+        <v>2</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>速度药水</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>15000034</v>
+        <v>15000035</v>
       </c>
       <c r="B36">
-        <v>22033014</v>
+        <v>22034008</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36">
-        <v>3</v>
-      </c>
-      <c r="E36" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机武器卡</v>
+        <v>2</v>
+      </c>
+      <c r="E36" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>幸运药水</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>15000035</v>
+        <v>15000036</v>
       </c>
       <c r="B37">
-        <v>22033015</v>
+        <v>22034009</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>3</v>
-      </c>
-      <c r="E37" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机魔法卡</v>
+        <v>2</v>
+      </c>
+      <c r="E37" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>暴击药水</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>15000036</v>
+        <v>15000037</v>
       </c>
       <c r="B38">
-        <v>22033018</v>
+        <v>22034001</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2624,17 +2602,17 @@
       <c r="D38">
         <v>3</v>
       </c>
-      <c r="E38" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-艾尔</v>
+      <c r="E38" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>经验之书</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>15000037</v>
+        <v>15000038</v>
       </c>
       <c r="B39">
-        <v>22033017</v>
+        <v>22034002</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2642,17 +2620,17 @@
       <c r="D39">
         <v>3</v>
       </c>
-      <c r="E39" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-普尔</v>
+      <c r="E39" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>能量之书</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>15000038</v>
+        <v>15000039</v>
       </c>
       <c r="B40">
-        <v>22033016</v>
+        <v>22034011</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2660,45 +2638,9 @@
       <c r="D40">
         <v>3</v>
       </c>
-      <c r="E40" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-查姆</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>15000039</v>
-      </c>
-      <c r="B41">
-        <v>22034001</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>3</v>
-      </c>
-      <c r="E41" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>经验之书</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>15000040</v>
-      </c>
-      <c r="B42">
-        <v>22034002</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>3</v>
-      </c>
-      <c r="E42" t="str">
-        <f>LOOKUP(表1[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>能量之书</v>
+      <c r="E40" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>体力药水</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#88 adjust the wheel cardbag->card only
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -36,9 +36,6 @@
     <t>ItemId</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -58,6 +55,10 @@
   </si>
   <si>
     <t>道具名</t>
+  </si>
+  <si>
+    <t>~Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1128,7 +1129,7 @@
             <v>22033030</v>
           </cell>
           <cell r="B44" t="str">
-            <v>小型药剂-命</v>
+            <v>木质修理锤</v>
           </cell>
         </row>
         <row r="45">
@@ -1136,7 +1137,7 @@
             <v>22033031</v>
           </cell>
           <cell r="B45" t="str">
-            <v>药剂-命</v>
+            <v>钢铁修理锤</v>
           </cell>
         </row>
         <row r="46">
@@ -1144,7 +1145,7 @@
             <v>22033032</v>
           </cell>
           <cell r="B46" t="str">
-            <v>大型药剂-命</v>
+            <v>神圣修理锤</v>
           </cell>
         </row>
         <row r="47">
@@ -1620,7 +1621,7 @@
     <tableColumn id="2" name="ItemId"/>
     <tableColumn id="3" name="Type"/>
     <tableColumn id="4" name="Shelf"/>
-    <tableColumn id="5" name="Name" dataDxfId="0">
+    <tableColumn id="5" name="~Name" dataDxfId="0">
       <calculatedColumnFormula>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1918,7 +1919,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1928,36 +1929,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1974,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2442,7 +2443,7 @@
       </c>
       <c r="E29" s="1" t="str">
         <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>药剂-命</v>
+        <v>钢铁修理锤</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2460,7 +2461,7 @@
       </c>
       <c r="E30" s="1" t="str">
         <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型药剂-命</v>
+        <v>神圣修理锤</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add some item to recover health and mental. quest of 1-2
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -1519,7 +1519,7 @@
             <v>22034010</v>
           </cell>
           <cell r="B85" t="str">
-            <v>生存药水</v>
+            <v>饼干</v>
           </cell>
         </row>
         <row r="86">
@@ -1527,86 +1527,94 @@
             <v>22034011</v>
           </cell>
           <cell r="B86" t="str">
-            <v>体力药水</v>
+            <v>红色胶囊</v>
           </cell>
         </row>
         <row r="87">
           <cell r="A87">
-            <v>22035001</v>
+            <v>22034012</v>
           </cell>
           <cell r="B87" t="str">
-            <v>猛兽卡片</v>
+            <v>蓝色胶囊</v>
           </cell>
         </row>
         <row r="88">
           <cell r="A88">
-            <v>22035002</v>
+            <v>22035001</v>
           </cell>
           <cell r="B88" t="str">
-            <v>战斧卡片</v>
+            <v>猛兽卡片</v>
           </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>22035003</v>
+            <v>22035002</v>
           </cell>
           <cell r="B89" t="str">
-            <v>火焰卡片</v>
+            <v>战斧卡片</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>22037001</v>
+            <v>22035003</v>
           </cell>
           <cell r="B90" t="str">
-            <v>种子-豌豆</v>
+            <v>火焰卡片</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>22037002</v>
+            <v>22037001</v>
           </cell>
           <cell r="B91" t="str">
-            <v>种子-玉米</v>
+            <v>种子-豌豆</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>22037003</v>
+            <v>22037002</v>
           </cell>
           <cell r="B92" t="str">
-            <v>种子-苹果</v>
+            <v>种子-玉米</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>22037004</v>
+            <v>22037003</v>
           </cell>
           <cell r="B93" t="str">
-            <v>种子-蓝莓</v>
+            <v>种子-苹果</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>22037101</v>
+            <v>22037004</v>
           </cell>
           <cell r="B94" t="str">
-            <v>作物-豌豆</v>
+            <v>种子-蓝莓</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>22037102</v>
+            <v>22037101</v>
           </cell>
           <cell r="B95" t="str">
-            <v>作物-玉米</v>
+            <v>作物-豌豆</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
+            <v>22037102</v>
+          </cell>
+          <cell r="B96" t="str">
+            <v>作物-玉米</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97">
             <v>22037103</v>
           </cell>
-          <cell r="B96" t="str">
+          <cell r="B97" t="str">
             <v>作物-苹果</v>
           </cell>
         </row>
@@ -1617,8 +1625,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D40" totalsRowShown="0">
-  <autoFilter ref="A3:D40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D42" totalsRowShown="0">
+  <autoFilter ref="A3:D42"/>
   <sortState ref="A4:E42">
     <sortCondition ref="A3:A42"/>
   </sortState>
@@ -1921,10 +1929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2519,14 +2527,44 @@
         <v>15000039</v>
       </c>
       <c r="B40">
-        <v>22034011</v>
+        <v>22034010</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
       <c r="D40" s="1" t="str">
         <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>体力药水</v>
+        <v>饼干</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>15000040</v>
+      </c>
+      <c r="B41">
+        <v>22034011</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>红色胶囊</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>15000041</v>
+      </c>
+      <c r="B42">
+        <v>22034012</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>蓝色胶囊</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change the icon of detect item
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -751,74 +751,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1540,81 +1472,89 @@
         </row>
         <row r="88">
           <cell r="A88">
-            <v>22035001</v>
+            <v>22034013</v>
           </cell>
           <cell r="B88" t="str">
-            <v>猛兽卡片</v>
+            <v>水晶球</v>
           </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>22035002</v>
+            <v>22035001</v>
           </cell>
           <cell r="B89" t="str">
-            <v>战斧卡片</v>
+            <v>猛兽卡片</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>22035003</v>
+            <v>22035002</v>
           </cell>
           <cell r="B90" t="str">
-            <v>火焰卡片</v>
+            <v>战斧卡片</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>22037001</v>
+            <v>22035003</v>
           </cell>
           <cell r="B91" t="str">
-            <v>种子-豌豆</v>
+            <v>火焰卡片</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>22037002</v>
+            <v>22037001</v>
           </cell>
           <cell r="B92" t="str">
-            <v>种子-玉米</v>
+            <v>种子-豌豆</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>22037003</v>
+            <v>22037002</v>
           </cell>
           <cell r="B93" t="str">
-            <v>种子-苹果</v>
+            <v>种子-玉米</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>22037004</v>
+            <v>22037003</v>
           </cell>
           <cell r="B94" t="str">
-            <v>种子-蓝莓</v>
+            <v>种子-苹果</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>22037101</v>
+            <v>22037004</v>
           </cell>
           <cell r="B95" t="str">
-            <v>作物-豌豆</v>
+            <v>种子-蓝莓</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>22037102</v>
+            <v>22037101</v>
           </cell>
           <cell r="B96" t="str">
-            <v>作物-玉米</v>
+            <v>作物-豌豆</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
+            <v>22037102</v>
+          </cell>
+          <cell r="B97" t="str">
+            <v>作物-玉米</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98">
             <v>22037103</v>
           </cell>
-          <cell r="B97" t="str">
+          <cell r="B98" t="str">
             <v>作物-苹果</v>
           </cell>
         </row>
@@ -1625,8 +1565,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D42" totalsRowShown="0">
-  <autoFilter ref="A3:D42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D43" totalsRowShown="0">
+  <autoFilter ref="A3:D43"/>
   <sortState ref="A4:E42">
     <sortCondition ref="A3:A42"/>
   </sortState>
@@ -1643,14 +1583,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1718,6 +1658,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1753,6 +1710,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1929,10 +1903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2567,6 +2541,21 @@
         <v>蓝色胶囊</v>
       </c>
     </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>15000042</v>
+      </c>
+      <c r="B43">
+        <v>22034013</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>水晶球</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add ranged move item and the move effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -1480,81 +1480,105 @@
         </row>
         <row r="89">
           <cell r="A89">
-            <v>22035001</v>
+            <v>22034014</v>
           </cell>
           <cell r="B89" t="str">
-            <v>猛兽卡片</v>
+            <v>坐骑黑豹</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>22035002</v>
+            <v>22034015</v>
           </cell>
           <cell r="B90" t="str">
-            <v>战斧卡片</v>
+            <v>坐骑鹰</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>22035003</v>
+            <v>22034016</v>
           </cell>
           <cell r="B91" t="str">
-            <v>火焰卡片</v>
+            <v>坐骑传送器</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>22037001</v>
+            <v>22035001</v>
           </cell>
           <cell r="B92" t="str">
-            <v>种子-豌豆</v>
+            <v>猛兽卡片</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>22037002</v>
+            <v>22035002</v>
           </cell>
           <cell r="B93" t="str">
-            <v>种子-玉米</v>
+            <v>战斧卡片</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>22037003</v>
+            <v>22035003</v>
           </cell>
           <cell r="B94" t="str">
-            <v>种子-苹果</v>
+            <v>火焰卡片</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>22037004</v>
+            <v>22037001</v>
           </cell>
           <cell r="B95" t="str">
-            <v>种子-蓝莓</v>
+            <v>种子-豌豆</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>22037101</v>
+            <v>22037002</v>
           </cell>
           <cell r="B96" t="str">
-            <v>作物-豌豆</v>
+            <v>种子-玉米</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>22037102</v>
+            <v>22037003</v>
           </cell>
           <cell r="B97" t="str">
-            <v>作物-玉米</v>
+            <v>种子-苹果</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
+            <v>22037004</v>
+          </cell>
+          <cell r="B98" t="str">
+            <v>种子-蓝莓</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99">
+            <v>22037101</v>
+          </cell>
+          <cell r="B99" t="str">
+            <v>作物-豌豆</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100">
+            <v>22037102</v>
+          </cell>
+          <cell r="B100" t="str">
+            <v>作物-玉米</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101">
             <v>22037103</v>
           </cell>
-          <cell r="B98" t="str">
+          <cell r="B101" t="str">
             <v>作物-苹果</v>
           </cell>
         </row>
@@ -1565,8 +1589,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D43" totalsRowShown="0">
-  <autoFilter ref="A3:D43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D46" totalsRowShown="0">
+  <autoFilter ref="A3:D46"/>
   <sortState ref="A4:E42">
     <sortCondition ref="A3:A42"/>
   </sortState>
@@ -1903,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2556,6 +2580,51 @@
         <v>水晶球</v>
       </c>
     </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>15000043</v>
+      </c>
+      <c r="B44">
+        <v>22034014</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>坐骑黑豹</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>15000044</v>
+      </c>
+      <c r="B45">
+        <v>22034015</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>坐骑鹰</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>15000045</v>
+      </c>
+      <c r="B46">
+        <v>22034016</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1" t="str">
+        <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>坐骑传送器</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
link the minigame with scenequest, and finish 2 game based scenequest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +220,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -663,7 +672,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -671,6 +680,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -808,138 +820,138 @@
         </row>
         <row r="5">
           <cell r="A5">
-            <v>22031002</v>
+            <v>22031101</v>
           </cell>
           <cell r="B5" t="str">
-            <v>卡牌补给包（无）</v>
+            <v>素材袋</v>
           </cell>
         </row>
         <row r="6">
           <cell r="A6">
-            <v>22031003</v>
+            <v>22031102</v>
           </cell>
           <cell r="B6" t="str">
-            <v>卡牌补给包（水）</v>
+            <v>高级素材袋</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7">
-            <v>22031004</v>
+            <v>22031103</v>
           </cell>
           <cell r="B7" t="str">
-            <v>卡牌补给包（风）</v>
+            <v>特级素材袋</v>
           </cell>
         </row>
         <row r="8">
           <cell r="A8">
-            <v>22031005</v>
+            <v>22031104</v>
           </cell>
           <cell r="B8" t="str">
-            <v>卡牌补给包（地）</v>
+            <v>极品素材袋</v>
           </cell>
         </row>
         <row r="9">
           <cell r="A9">
-            <v>22031006</v>
+            <v>22031201</v>
           </cell>
           <cell r="B9" t="str">
-            <v>卡牌补给包（火）</v>
+            <v>蓝色卡包</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10">
-            <v>22031007</v>
+            <v>22031202</v>
           </cell>
           <cell r="B10" t="str">
-            <v>卡牌补给包（光）</v>
+            <v>黄色卡包</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11">
-            <v>22031008</v>
+            <v>22031203</v>
           </cell>
           <cell r="B11" t="str">
-            <v>卡牌补给包（暗）</v>
+            <v>红色卡包</v>
           </cell>
         </row>
         <row r="12">
           <cell r="A12">
-            <v>22031011</v>
+            <v>22031212</v>
           </cell>
           <cell r="B12" t="str">
-            <v>卡牌补给包（生物）</v>
+            <v>卡牌补给包（无）</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13">
-            <v>22031012</v>
+            <v>22031213</v>
           </cell>
           <cell r="B13" t="str">
-            <v>卡牌补给包（武器）</v>
+            <v>卡牌补给包（水）</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14">
-            <v>22031013</v>
+            <v>22031214</v>
           </cell>
           <cell r="B14" t="str">
-            <v>卡牌补给包（法术）</v>
+            <v>卡牌补给包（风）</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15">
-            <v>22031101</v>
+            <v>22031215</v>
           </cell>
           <cell r="B15" t="str">
-            <v>素材袋</v>
+            <v>卡牌补给包（地）</v>
           </cell>
         </row>
         <row r="16">
           <cell r="A16">
-            <v>22031102</v>
+            <v>22031216</v>
           </cell>
           <cell r="B16" t="str">
-            <v>高级素材袋</v>
+            <v>卡牌补给包（火）</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17">
-            <v>22031103</v>
+            <v>22031217</v>
           </cell>
           <cell r="B17" t="str">
-            <v>特级素材袋</v>
+            <v>卡牌补给包（光）</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18">
-            <v>22031104</v>
+            <v>22031218</v>
           </cell>
           <cell r="B18" t="str">
-            <v>极品素材袋</v>
+            <v>卡牌补给包（暗）</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19">
-            <v>22031201</v>
+            <v>22031221</v>
           </cell>
           <cell r="B19" t="str">
-            <v>蓝色卡包</v>
+            <v>卡牌补给包（生物）</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20">
-            <v>22031202</v>
+            <v>22031222</v>
           </cell>
           <cell r="B20" t="str">
-            <v>黄色卡包</v>
+            <v>卡牌补给包（武器）</v>
           </cell>
         </row>
         <row r="21">
           <cell r="A21">
-            <v>22031203</v>
+            <v>22031223</v>
           </cell>
           <cell r="B21" t="str">
-            <v>红色卡包</v>
+            <v>卡牌补给包（法术）</v>
           </cell>
         </row>
         <row r="22">
@@ -1504,81 +1516,57 @@
         </row>
         <row r="92">
           <cell r="A92">
-            <v>22035001</v>
+            <v>22037001</v>
           </cell>
           <cell r="B92" t="str">
-            <v>猛兽卡片</v>
+            <v>种子-豌豆</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>22035002</v>
+            <v>22037002</v>
           </cell>
           <cell r="B93" t="str">
-            <v>战斧卡片</v>
+            <v>种子-玉米</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>22035003</v>
+            <v>22037003</v>
           </cell>
           <cell r="B94" t="str">
-            <v>火焰卡片</v>
+            <v>种子-苹果</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>22037001</v>
+            <v>22037004</v>
           </cell>
           <cell r="B95" t="str">
-            <v>种子-豌豆</v>
+            <v>种子-蓝莓</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>22037002</v>
+            <v>22037101</v>
           </cell>
           <cell r="B96" t="str">
-            <v>种子-玉米</v>
+            <v>作物-豌豆</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>22037003</v>
+            <v>22037102</v>
           </cell>
           <cell r="B97" t="str">
-            <v>种子-苹果</v>
+            <v>作物-玉米</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>22037004</v>
+            <v>22037103</v>
           </cell>
           <cell r="B98" t="str">
-            <v>种子-蓝莓</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99">
-            <v>22037101</v>
-          </cell>
-          <cell r="B99" t="str">
-            <v>作物-豌豆</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100">
-            <v>22037102</v>
-          </cell>
-          <cell r="B100" t="str">
-            <v>作物-玉米</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="A101">
-            <v>22037103</v>
-          </cell>
-          <cell r="B101" t="str">
             <v>作物-苹果</v>
           </cell>
         </row>
@@ -1929,8 +1917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1938,17 +1926,17 @@
     <col min="1" max="2" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1985,14 +1973,14 @@
         <v>15000001</v>
       </c>
       <c r="B4">
-        <v>22035001</v>
+        <v>22031201</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>猛兽卡片</v>
+        <v>蓝色卡包</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -2000,14 +1988,14 @@
         <v>15000002</v>
       </c>
       <c r="B5">
-        <v>22035002</v>
+        <v>22031202</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="str">
         <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>战斧卡片</v>
+        <v>黄色卡包</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -2015,14 +2003,14 @@
         <v>15000003</v>
       </c>
       <c r="B6">
-        <v>22035003</v>
+        <v>22031203</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="str">
         <f>LOOKUP(表3[[#This Row],[ItemId]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>火焰卡片</v>
+        <v>红色卡包</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -2030,7 +2018,7 @@
         <v>15000004</v>
       </c>
       <c r="B7">
-        <v>22031002</v>
+        <v>22031212</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2045,7 +2033,7 @@
         <v>15000005</v>
       </c>
       <c r="B8">
-        <v>22031003</v>
+        <v>22031213</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2060,7 +2048,7 @@
         <v>15000006</v>
       </c>
       <c r="B9">
-        <v>22031004</v>
+        <v>22031214</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2075,7 +2063,7 @@
         <v>15000007</v>
       </c>
       <c r="B10">
-        <v>22031005</v>
+        <v>22031215</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2090,7 +2078,7 @@
         <v>15000008</v>
       </c>
       <c r="B11">
-        <v>22031006</v>
+        <v>22031216</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2105,7 +2093,7 @@
         <v>15000009</v>
       </c>
       <c r="B12">
-        <v>22031007</v>
+        <v>22031217</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2120,7 +2108,7 @@
         <v>15000010</v>
       </c>
       <c r="B13">
-        <v>22031008</v>
+        <v>22031218</v>
       </c>
       <c r="C13">
         <v>1</v>

</xml_diff>

<commit_message>
remake the effect of drugs
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -117,27 +117,6 @@
     <t>shenshengxiulichui</t>
   </si>
   <si>
-    <t>gongsuyaoshui</t>
-  </si>
-  <si>
-    <t>shouhuyaoshui</t>
-  </si>
-  <si>
-    <t>fashuyaoshui</t>
-  </si>
-  <si>
-    <t>jiqiaoyaoshui</t>
-  </si>
-  <si>
-    <t>suduyaoshui</t>
-  </si>
-  <si>
-    <t>xingyunyaoshui</t>
-  </si>
-  <si>
-    <t>baojiyaoshui</t>
-  </si>
-  <si>
     <t>jingyanzhishu</t>
   </si>
   <si>
@@ -171,6 +150,34 @@
   </si>
   <si>
     <t>装备/道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaoshuistr</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaoshuiintl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaoshui1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaoshui2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaoshuiagi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaoshuiperc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaoshuiendu</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -536,7 +543,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -651,6 +658,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -780,7 +796,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -789,6 +805,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -851,8 +870,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:C45" totalsRowShown="0">
   <autoFilter ref="A3:C45"/>
-  <sortState ref="A4:D42">
-    <sortCondition ref="A3:A42"/>
+  <sortState ref="A4:D35">
+    <sortCondition ref="A3:A35"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Id"/>
@@ -1186,13 +1205,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1200,7 +1220,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
@@ -1211,7 +1231,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -1222,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1439,7 +1459,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>15000021</v>
+        <v>15000020</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -1450,7 +1470,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>15000022</v>
+        <v>15000021</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -1461,7 +1481,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>15000024</v>
+        <v>15000022</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -1472,7 +1492,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>15000025</v>
+        <v>15000023</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -1483,7 +1503,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>15000026</v>
+        <v>15000024</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -1494,7 +1514,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>15000027</v>
+        <v>15000025</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -1505,7 +1525,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>15000028</v>
+        <v>15000026</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -1516,7 +1536,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>15000029</v>
+        <v>15000027</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -1527,84 +1547,84 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>15000030</v>
+        <v>15000028</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>15000031</v>
+        <v>15000029</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>15000032</v>
+        <v>15000030</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>15000033</v>
+        <v>15000031</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>15000034</v>
+        <v>15000032</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>15000035</v>
+        <v>15000033</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>15000036</v>
+        <v>15000034</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>15000037</v>
+        <v>15000035</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -1615,10 +1635,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>15000038</v>
-      </c>
-      <c r="B39" t="s">
-        <v>40</v>
+        <v>15000036</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -1626,10 +1646,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>15000039</v>
-      </c>
-      <c r="B40" t="s">
-        <v>41</v>
+        <v>15000037</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -1637,10 +1657,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>15000040</v>
-      </c>
-      <c r="B41" t="s">
-        <v>42</v>
+        <v>15000038</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -1648,10 +1668,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>15000041</v>
-      </c>
-      <c r="B42" t="s">
-        <v>43</v>
+        <v>15000039</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C42">
         <v>3</v>
@@ -1659,10 +1679,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43">
-        <v>15000042</v>
-      </c>
-      <c r="B43" t="s">
-        <v>44</v>
+        <v>15000040</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C43">
         <v>3</v>
@@ -1670,10 +1690,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>15000043</v>
-      </c>
-      <c r="B44" t="s">
-        <v>45</v>
+        <v>15000041</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C44">
         <v>3</v>
@@ -1681,10 +1701,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45">
-        <v>15000044</v>
-      </c>
-      <c r="B45" t="s">
-        <v>46</v>
+        <v>15000042</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C45">
         <v>3</v>

</xml_diff>

<commit_message>
optimise the card bag in game shop
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Shelf</t>
   </si>
@@ -34,45 +34,6 @@
   </si>
   <si>
     <t>货架id</t>
-  </si>
-  <si>
-    <t>kabaolanse</t>
-  </si>
-  <si>
-    <t>kabaohuangse</t>
-  </si>
-  <si>
-    <t>kabaohongse</t>
-  </si>
-  <si>
-    <t>kapaibugeibao(wu)</t>
-  </si>
-  <si>
-    <t>kapaibugeibao(shui)</t>
-  </si>
-  <si>
-    <t>kapaibugeibao(feng)</t>
-  </si>
-  <si>
-    <t>kapaibugeibao(di)</t>
-  </si>
-  <si>
-    <t>kapaibugeibao(huo)</t>
-  </si>
-  <si>
-    <t>kapaibugeibao(guang)</t>
-  </si>
-  <si>
-    <t>kapaibugeibao(an)</t>
-  </si>
-  <si>
-    <t>sucaidai</t>
-  </si>
-  <si>
-    <t>sucaidaigaoji</t>
-  </si>
-  <si>
-    <t>sucaidaiteji</t>
   </si>
   <si>
     <t>suijihuanshouka</t>
@@ -178,6 +139,18 @@
   </si>
   <si>
     <t>yaoshuiendu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kabao1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kabao1v2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kabao1v3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -868,10 +841,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:C45" totalsRowShown="0">
-  <autoFilter ref="A3:C45"/>
-  <sortState ref="A4:D35">
-    <sortCondition ref="A3:A35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:C35" totalsRowShown="0">
+  <autoFilter ref="A3:C35"/>
+  <sortState ref="A4:D25">
+    <sortCondition ref="A3:A25"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Id"/>
@@ -1203,9 +1176,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1220,7 +1193,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
@@ -1231,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -1242,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1253,7 +1226,7 @@
         <v>15000001</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1264,7 +1237,7 @@
         <v>15000002</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1275,7 +1248,7 @@
         <v>15000003</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1283,120 +1256,120 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>15000004</v>
+        <v>15000014</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>15000005</v>
+        <v>15000015</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>15000006</v>
+        <v>15000016</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>15000007</v>
+        <v>15000017</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>15000008</v>
+        <v>15000018</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>15000009</v>
+        <v>15000019</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>15000010</v>
+        <v>15000020</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>15000011</v>
+        <v>15000021</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>15000012</v>
+        <v>15000022</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>15000013</v>
+        <v>15000023</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>15000014</v>
+        <v>15000024</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1404,10 +1377,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>15000015</v>
+        <v>15000025</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1415,10 +1388,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>15000016</v>
+        <v>15000026</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1426,10 +1399,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>15000017</v>
+        <v>15000027</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1437,119 +1410,119 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>15000018</v>
+        <v>15000028</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>15000019</v>
+        <v>15000029</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>15000020</v>
+        <v>15000030</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>15000021</v>
+        <v>15000031</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>15000022</v>
+        <v>15000032</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>15000023</v>
+        <v>15000033</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>15000024</v>
+        <v>15000034</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>15000025</v>
+        <v>15000035</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>15000026</v>
-      </c>
-      <c r="B29" t="s">
+        <v>15000036</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>15000027</v>
-      </c>
-      <c r="B30" t="s">
+        <v>15000037</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>15000028</v>
-      </c>
-      <c r="B31" t="s">
+        <v>15000038</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C31">
@@ -1558,9 +1531,9 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>15000029</v>
-      </c>
-      <c r="B32" t="s">
+        <v>15000039</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C32">
@@ -1569,9 +1542,9 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>15000030</v>
-      </c>
-      <c r="B33" t="s">
+        <v>15000040</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C33">
@@ -1580,9 +1553,9 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>15000031</v>
-      </c>
-      <c r="B34" t="s">
+        <v>15000041</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C34">
@@ -1591,122 +1564,12 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>15000032</v>
-      </c>
-      <c r="B35" t="s">
+        <v>15000042</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36">
-        <v>15000033</v>
-      </c>
-      <c r="B36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37">
-        <v>15000034</v>
-      </c>
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38">
-        <v>15000035</v>
-      </c>
-      <c r="B38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39">
-        <v>15000036</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40">
-        <v>15000037</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41">
-        <v>15000038</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42">
-        <v>15000039</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43">
-        <v>15000040</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44">
-        <v>15000041</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45">
-        <v>15000042</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
support gold buy item in game shop
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Shelf</t>
   </si>
@@ -151,6 +151,26 @@
   </si>
   <si>
     <t>kabao1v3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>钻石购买</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>UseDiamond</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -769,7 +789,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -780,6 +800,9 @@
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -827,7 +850,11 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -841,15 +868,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:C35" totalsRowShown="0">
-  <autoFilter ref="A3:C35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D35" totalsRowShown="0">
+  <autoFilter ref="A3:D35"/>
   <sortState ref="A4:D25">
     <sortCondition ref="A3:A25"/>
   </sortState>
-  <tableColumns count="3">
+  <tableColumns count="4">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Item"/>
     <tableColumn id="4" name="Shelf"/>
+    <tableColumn id="3" name="UseDiamond" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1176,19 +1204,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.625" customWidth="1"/>
+    <col min="3" max="3" width="5.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1198,8 +1227,11 @@
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1209,8 +1241,11 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1220,8 +1255,11 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>15000001</v>
       </c>
@@ -1231,8 +1269,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D4" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>15000002</v>
       </c>
@@ -1242,8 +1283,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D5" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>15000003</v>
       </c>
@@ -1253,8 +1297,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>15000014</v>
       </c>
@@ -1264,8 +1311,11 @@
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D7" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>15000015</v>
       </c>
@@ -1275,8 +1325,11 @@
       <c r="C8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>15000016</v>
       </c>
@@ -1286,8 +1339,11 @@
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D9" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>15000017</v>
       </c>
@@ -1297,8 +1353,11 @@
       <c r="C10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D10" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>15000018</v>
       </c>
@@ -1308,8 +1367,11 @@
       <c r="C11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D11" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>15000019</v>
       </c>
@@ -1319,8 +1381,11 @@
       <c r="C12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D12" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>15000020</v>
       </c>
@@ -1330,8 +1395,11 @@
       <c r="C13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>15000021</v>
       </c>
@@ -1341,8 +1409,11 @@
       <c r="C14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>15000022</v>
       </c>
@@ -1352,8 +1423,11 @@
       <c r="C15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D15" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15000023</v>
       </c>
@@ -1363,8 +1437,11 @@
       <c r="C16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D16" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>15000024</v>
       </c>
@@ -1374,8 +1451,11 @@
       <c r="C17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D17" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>15000025</v>
       </c>
@@ -1385,8 +1465,11 @@
       <c r="C18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D18" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>15000026</v>
       </c>
@@ -1396,8 +1479,11 @@
       <c r="C19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D19" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>15000027</v>
       </c>
@@ -1407,8 +1493,11 @@
       <c r="C20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D20" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>15000028</v>
       </c>
@@ -1418,8 +1507,11 @@
       <c r="C21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D21" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>15000029</v>
       </c>
@@ -1429,8 +1521,11 @@
       <c r="C22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D22" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>15000030</v>
       </c>
@@ -1440,8 +1535,11 @@
       <c r="C23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D23" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>15000031</v>
       </c>
@@ -1451,8 +1549,11 @@
       <c r="C24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D24" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>15000032</v>
       </c>
@@ -1462,8 +1563,11 @@
       <c r="C25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D25" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>15000033</v>
       </c>
@@ -1473,8 +1577,11 @@
       <c r="C26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D26" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>15000034</v>
       </c>
@@ -1484,8 +1591,11 @@
       <c r="C27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D27" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>15000035</v>
       </c>
@@ -1495,8 +1605,11 @@
       <c r="C28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D28" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>15000036</v>
       </c>
@@ -1506,8 +1619,11 @@
       <c r="C29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D29" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>15000037</v>
       </c>
@@ -1517,8 +1633,11 @@
       <c r="C30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D30" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>15000038</v>
       </c>
@@ -1528,8 +1647,11 @@
       <c r="C31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D31" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>15000039</v>
       </c>
@@ -1539,8 +1661,11 @@
       <c r="C32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D32" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>15000040</v>
       </c>
@@ -1550,8 +1675,11 @@
       <c r="C33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D33" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>15000041</v>
       </c>
@@ -1561,8 +1689,11 @@
       <c r="C34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D34" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>15000042</v>
       </c>
@@ -1571,6 +1702,9 @@
       </c>
       <c r="C35">
         <v>3</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add ep by item
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F6698879-6EEE-4BDA-AA38-64C21C01ED83}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GameShop" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t>Shelf</t>
   </si>
@@ -172,12 +173,15 @@
   <si>
     <t>false</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jueyu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -868,16 +872,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D35" totalsRowShown="0">
-  <autoFilter ref="A3:D35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:D36" totalsRowShown="0">
+  <autoFilter ref="A3:D36" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState ref="A4:D25">
     <sortCondition ref="A3:A25"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="Item"/>
-    <tableColumn id="4" name="Shelf"/>
-    <tableColumn id="3" name="UseDiamond" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Item"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Shelf"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="UseDiamond" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1203,11 +1207,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1613,8 +1617,8 @@
       <c r="A29">
         <v>15000036</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>30</v>
+      <c r="B29" t="s">
+        <v>45</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1628,7 +1632,7 @@
         <v>15000037</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1642,7 +1646,7 @@
         <v>15000038</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -1656,7 +1660,7 @@
         <v>15000039</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -1670,7 +1674,7 @@
         <v>15000040</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -1684,7 +1688,7 @@
         <v>15000041</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -1698,12 +1702,26 @@
         <v>15000042</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35">
         <v>3</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>15000043</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new ep refresh item
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/GameShop.xlsx
+++ b/ConfigData/Xlsx/GameShop.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Shelf</t>
   </si>
@@ -179,6 +179,9 @@
   <si>
     <t>fuwen-aide</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuwen-aisi</t>
   </si>
 </sst>
 </file>
@@ -943,10 +946,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D37" totalsRowShown="0">
-  <autoFilter ref="A3:D37"/>
-  <sortState ref="A4:D26">
-    <sortCondition ref="A3:A26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D38" totalsRowShown="0">
+  <autoFilter ref="A3:D38"/>
+  <sortState ref="A4:D27">
+    <sortCondition ref="A3:A27"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Id"/>
@@ -1279,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1479,7 +1482,7 @@
         <v>15000021</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1493,7 +1496,7 @@
         <v>15000022</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1507,7 +1510,7 @@
         <v>15000023</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1521,7 +1524,7 @@
         <v>15000024</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1535,7 +1538,7 @@
         <v>15000025</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1549,7 +1552,7 @@
         <v>15000026</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1563,7 +1566,7 @@
         <v>15000027</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1577,7 +1580,7 @@
         <v>15000028</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1591,10 +1594,10 @@
         <v>15000029</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>43</v>
@@ -1605,7 +1608,7 @@
         <v>15000030</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -1619,7 +1622,7 @@
         <v>15000031</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -1633,7 +1636,7 @@
         <v>15000032</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1647,7 +1650,7 @@
         <v>15000033</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1661,7 +1664,7 @@
         <v>15000034</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -1675,7 +1678,7 @@
         <v>15000035</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -1689,7 +1692,7 @@
         <v>15000036</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1703,7 +1706,7 @@
         <v>15000037</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1716,8 +1719,8 @@
       <c r="A31">
         <v>15000038</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>30</v>
+      <c r="B31" t="s">
+        <v>45</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -1731,7 +1734,7 @@
         <v>15000039</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -1745,7 +1748,7 @@
         <v>15000040</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -1759,7 +1762,7 @@
         <v>15000041</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -1773,7 +1776,7 @@
         <v>15000042</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -1787,7 +1790,7 @@
         <v>15000043</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36">
         <v>3</v>
@@ -1801,12 +1804,26 @@
         <v>15000044</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>15000045</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>